<commit_message>
adding project files ssis ssas and screenshots
</commit_message>
<xml_diff>
--- a/Important_Docs/DWH Fact and Dimensions.xlsx
+++ b/Important_Docs/DWH Fact and Dimensions.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\drive-download-20191524997\My_Profile\MyOwnProjects\Garvity_Books\GravityBooks_DWH\Important_Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Computec\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1875C398-E4BB-428A-A0D3-F1895A398E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAB2380-D206-48BB-9366-A8A4890DE5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="2064" windowWidth="18216" windowHeight="10248" xr2:uid="{A8F2234F-CC56-4504-A498-5AD9EC18B1F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{A8F2234F-CC56-4504-A498-5AD9EC18B1F1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Fact &amp; Dimensions" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>book_dim</t>
   </si>
@@ -60,9 +60,6 @@
     <t>author_name</t>
   </si>
   <si>
-    <t xml:space="preserve">price </t>
-  </si>
-  <si>
     <t xml:space="preserve">publication_date </t>
   </si>
   <si>
@@ -84,18 +81,6 @@
     <t>Customer_Bk</t>
   </si>
   <si>
-    <t xml:space="preserve">Full_name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">email </t>
-  </si>
-  <si>
-    <t>Streat_name</t>
-  </si>
-  <si>
-    <t>street_number</t>
-  </si>
-  <si>
     <t xml:space="preserve">City </t>
   </si>
   <si>
@@ -123,18 +108,9 @@
     <t xml:space="preserve">Status_Value </t>
   </si>
   <si>
-    <t xml:space="preserve">Status_date </t>
-  </si>
-  <si>
-    <t xml:space="preserve">order_date </t>
-  </si>
-  <si>
     <t xml:space="preserve"> FactTable</t>
   </si>
   <si>
-    <t>Custdim_sk_Fk int NOT NULL,</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fact_sk </t>
   </si>
   <si>
@@ -153,20 +129,53 @@
     <t>number of pages</t>
   </si>
   <si>
-    <t xml:space="preserve">price(total price)  </t>
-  </si>
-  <si>
     <t>method_id</t>
   </si>
   <si>
     <t>line_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custdim_sk_Fk </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price(Sales)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last_name </t>
+  </si>
+  <si>
+    <t>First_name</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>Date_Dim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date_sk </t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Quarter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,8 +183,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,43 +200,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -237,18 +241,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -267,9 +277,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -307,7 +317,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -413,7 +423,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -555,208 +565,245 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79BC3CA6-B4E0-4BA5-811A-14AE1D9E2762}">
-  <dimension ref="A2:L20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF12EA86-7288-4AB4-AA08-C98A698E0E9A}">
+  <dimension ref="C3:L33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="14.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="8.7265625" style="1"/>
+    <col min="8" max="8" width="23.90625" style="1" customWidth="1"/>
+    <col min="9" max="11" width="8.7265625" style="1"/>
+    <col min="12" max="12" width="15" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H3" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H4" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H5" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H6" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H7" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H8" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H9" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="12" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="s">
+    </row>
+    <row r="14" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D24" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H25" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H26" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H27" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H28" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H29" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="L8" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
+    <row r="30" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H30" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="6" t="s">
+    </row>
+    <row r="31" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H31" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="6" t="s">
+    </row>
+    <row r="32" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="H32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="G20" s="7"/>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>